<commit_message>
Finished HQ scores output script
</commit_message>
<xml_diff>
--- a/Data/ReachInfo.xlsx
+++ b/Data/ReachInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0166AED-D3BD-4C4E-B6DB-B53DD26F3AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF189587-791C-40D4-8FD8-AF604AAEB80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="504" yWindow="204" windowWidth="22536" windowHeight="12120" xr2:uid="{A4648F98-2B95-4B22-87B5-21156F112F0F}"/>
+    <workbookView xWindow="2148" yWindow="504" windowWidth="19644" windowHeight="11340" xr2:uid="{A4648F98-2B95-4B22-87B5-21156F112F0F}"/>
   </bookViews>
   <sheets>
     <sheet name="ReachInfo" sheetId="2" r:id="rId1"/>
@@ -7641,7 +7641,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>